<commit_message>
Refactor main.py and process_dataset.py: add new functions for data processing, enhance color mapping, and improve error handling
</commit_message>
<xml_diff>
--- a/notebooks/mupe_train_sample_postprocessed_final.xlsx
+++ b/notebooks/mupe_train_sample_postprocessed_final.xlsx
@@ -38,127 +38,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0049006A"/>
+        <fgColor rgb="00E41A1C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0059006E"/>
+        <fgColor rgb="00377EB8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="006A0173"/>
+        <fgColor rgb="004DAF4A"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="007A0177"/>
+        <fgColor rgb="00984EA3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="008B0179"/>
+        <fgColor rgb="00FF7F00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="009D017C"/>
+        <fgColor rgb="00FFFF33"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00AE017E"/>
+        <fgColor rgb="00A65628"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00BE1286"/>
+        <fgColor rgb="00F781BF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CD238F"/>
+        <fgColor rgb="00999999"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00DD3497"/>
+        <fgColor rgb="0066C2A5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E6459A"/>
+        <fgColor rgb="00FC8D62"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00EE579E"/>
+        <fgColor rgb="008DA0CB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F768A1"/>
+        <fgColor rgb="00E78AC3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F87AA8"/>
+        <fgColor rgb="00A6D854"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F98DAE"/>
+        <fgColor rgb="00FFD92F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FA9FB5"/>
+        <fgColor rgb="00E5C494"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FBACB9"/>
+        <fgColor rgb="00B3B3B3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FBB8BC"/>
+        <fgColor rgb="001B9E77"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FCC5C0"/>
+        <fgColor rgb="00D95F02"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FCCECA"/>
+        <fgColor rgb="007570B3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FDD7D3"/>
+        <fgColor rgb="00E7298A"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FDE0DD"/>
+        <fgColor rgb="0066A61E"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FEE8E4"/>
+        <fgColor rgb="00E6AB02"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FEEFEC"/>
+        <fgColor rgb="00A6761D"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFF7F3"/>
+        <fgColor rgb="00666666"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>